<commit_message>
[DOC] : Version Control Tool_Manual : SVN manual 초안 추가
</commit_message>
<xml_diff>
--- a/Version Control Tool_Manual_v1.0.xlsx
+++ b/Version Control Tool_Manual_v1.0.xlsx
@@ -4,24 +4,26 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GitHub 가입" sheetId="13" r:id="rId1"/>
     <sheet name="GitHub Local 설정" sheetId="14" r:id="rId2"/>
     <sheet name="Commit Log 확인 방법" sheetId="15" r:id="rId3"/>
+    <sheet name="TortoiseSVN" sheetId="16" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Commit Log 확인 방법'!$A$1:$N$147</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'GitHub Local 설정'!$A$1:$L$320</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'GitHub 가입'!$A$1:$P$140</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">TortoiseSVN!$A$1:$P$94</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>5. Repository 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -216,6 +218,26 @@
   </si>
   <si>
     <t>4. 이후 SourceTree를 사용하여 Git 관리(commit, push, pull)가 가능한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문서 관리 Tool 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. https://tortoisesvn.net/downloads.html 에서 TortoiseSVN 최신 version을 Download하여 Install 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Local에 SVN server로 사용할 folder(MP1_Data)를 생성한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. MP1_Data folder를 선택 후 Mouse Popup에서 TortoiseSVN -&gt; Create repository here를 차례로 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 아래와 같이 MP1_Data folder에서 하위 파일들이 생성되고, Popup 창이 실행되면 OK를 선택한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -223,7 +245,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +298,13 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -291,18 +323,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="쉼표 [0]" xfId="2" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
@@ -2880,6 +2918,409 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>596828</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="그룹 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1123950" y="704850"/>
+          <a:ext cx="7426253" cy="3648075"/>
+          <a:chOff x="1123950" y="704850"/>
+          <a:chExt cx="7426253" cy="3648075"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="그림 2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1123950" y="704850"/>
+            <a:ext cx="7426253" cy="3648075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6629400" y="3790949"/>
+            <a:ext cx="1295400" cy="390525"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9267825" y="9658349"/>
+          <a:ext cx="1295400" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="그룹 14"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1200150" y="4943475"/>
+          <a:ext cx="4791075" cy="3105150"/>
+          <a:chOff x="1200150" y="4943475"/>
+          <a:chExt cx="4791075" cy="3105150"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="14" name="그림 13"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1200150" y="4943475"/>
+            <a:ext cx="4791075" cy="3105150"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1476375" y="6943724"/>
+            <a:ext cx="2971800" cy="600076"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>120482</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="그림 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085851" y="8505825"/>
+          <a:ext cx="7353300" cy="4616282"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>63518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="그림 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1123950" y="13716000"/>
+          <a:ext cx="7400925" cy="3749693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -3431,7 +3872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
@@ -3492,4 +3933,62 @@
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:X71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U80" sqref="U80"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="4.625" customWidth="1"/>
+    <col min="20" max="20" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="T68" s="5"/>
+    </row>
+    <row r="71" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="T71" s="6"/>
+      <c r="X71" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="16" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[DOC] : Version Control Tool_Manual : GitHub Clone 설정 부분 수정
</commit_message>
<xml_diff>
--- a/Version Control Tool_Manual_v1.0.xlsx
+++ b/Version Control Tool_Manual_v1.0.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GitHub 가입" sheetId="13" r:id="rId1"/>
@@ -14,16 +14,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Commit Log 확인 방법'!$A$1:$N$147</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'GitHub Local 설정'!$A$1:$L$320</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'GitHub Local 설정'!$A$1:$L$321</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'GitHub 가입'!$A$1:$P$140</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">TortoiseSVN!$A$1:$P$94</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>5. Repository 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -238,6 +238,10 @@
   </si>
   <si>
     <t>4. 아래와 같이 MP1_Data folder에서 하위 파일들이 생성되고, Popup 창이 실행되면 OK를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clone 설정시 Clone folder는 비어 있어야 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -649,13 +653,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>74545</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>57979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>463827</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>211334</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -704,13 +708,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>66260</xdr:colOff>
-      <xdr:row>153</xdr:row>
+      <xdr:row>154</xdr:row>
       <xdr:rowOff>82826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>457664</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>198782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -759,14 +763,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>24021</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>81169</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>488675</xdr:colOff>
-      <xdr:row>192</xdr:row>
-      <xdr:rowOff>202222</xdr:rowOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>202223</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -814,13 +818,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>108088</xdr:colOff>
-      <xdr:row>280</xdr:row>
+      <xdr:row>281</xdr:row>
       <xdr:rowOff>89453</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>403363</xdr:colOff>
-      <xdr:row>300</xdr:row>
+      <xdr:row>301</xdr:row>
       <xdr:rowOff>159439</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1301,13 +1305,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>65941</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>87923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>273293</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>164123</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1317,8 +1321,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="670571" y="12147401"/>
-          <a:ext cx="3644635" cy="4598505"/>
+          <a:off x="670571" y="12362749"/>
+          <a:ext cx="3644635" cy="4598504"/>
           <a:chOff x="666749" y="12411808"/>
           <a:chExt cx="3651006" cy="4538296"/>
         </a:xfrm>
@@ -1415,13 +1419,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>92702</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>76774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>505239</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>150541</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1431,7 +1435,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="697332" y="17735296"/>
+          <a:off x="697332" y="17950644"/>
           <a:ext cx="4537277" cy="3303984"/>
           <a:chOff x="697332" y="18505578"/>
           <a:chExt cx="4537277" cy="3179746"/>
@@ -1574,13 +1578,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>99392</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>82827</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>405848</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>121674</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1590,7 +1594,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="704022" y="25709218"/>
+          <a:off x="704022" y="25924566"/>
           <a:ext cx="5806109" cy="2623021"/>
           <a:chOff x="704022" y="25493870"/>
           <a:chExt cx="5806109" cy="2623021"/>
@@ -1688,13 +1692,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>99393</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>91110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>115958</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>151</xdr:row>
       <xdr:rowOff>47375</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1704,7 +1708,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="704023" y="28947719"/>
+          <a:off x="704023" y="29163067"/>
           <a:ext cx="3453848" cy="3401830"/>
           <a:chOff x="1076740" y="28748936"/>
           <a:chExt cx="3453848" cy="3401830"/>
@@ -1802,13 +1806,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>197</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>91108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>231913</xdr:colOff>
-      <xdr:row>214</xdr:row>
+      <xdr:row>215</xdr:row>
       <xdr:rowOff>53483</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1818,7 +1822,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="753717" y="42514630"/>
+          <a:off x="753717" y="42729978"/>
           <a:ext cx="3520109" cy="3623288"/>
           <a:chOff x="687456" y="42357261"/>
           <a:chExt cx="4620040" cy="4755460"/>
@@ -1916,13 +1920,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>134179</xdr:colOff>
-      <xdr:row>256</xdr:row>
+      <xdr:row>257</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>173934</xdr:colOff>
-      <xdr:row>275</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>182218</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1932,7 +1936,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="738809" y="55214769"/>
+          <a:off x="738809" y="55430117"/>
           <a:ext cx="5539408" cy="4188101"/>
           <a:chOff x="713961" y="46559443"/>
           <a:chExt cx="4835387" cy="3650250"/>
@@ -2030,13 +2034,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>162341</xdr:colOff>
-      <xdr:row>216</xdr:row>
+      <xdr:row>217</xdr:row>
       <xdr:rowOff>72473</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>16565</xdr:colOff>
-      <xdr:row>234</xdr:row>
+      <xdr:row>235</xdr:row>
       <xdr:rowOff>149087</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2046,7 +2050,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="766971" y="46587603"/>
+          <a:off x="766971" y="46802951"/>
           <a:ext cx="5353877" cy="3952875"/>
           <a:chOff x="766971" y="46372256"/>
           <a:chExt cx="4835387" cy="3650250"/>
@@ -2144,13 +2148,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>168552</xdr:colOff>
-      <xdr:row>237</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>70402</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>103946</xdr:colOff>
-      <xdr:row>253</xdr:row>
+      <xdr:row>254</xdr:row>
       <xdr:rowOff>140805</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2160,7 +2164,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="773182" y="51107837"/>
+          <a:off x="773182" y="51323185"/>
           <a:ext cx="5435047" cy="3515968"/>
           <a:chOff x="773182" y="50892489"/>
           <a:chExt cx="5435047" cy="3515968"/>
@@ -3364,7 +3368,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3399,7 +3403,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3691,10 +3695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D307"/>
+  <dimension ref="B1:D308"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="N179" sqref="N179"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A133" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3744,113 +3748,118 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C80" t="s">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D81" t="s">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D82" t="s">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C99" t="s">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C118" t="s">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C119" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D119" t="s">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D120" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C134" t="s">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C135" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C153" t="s">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C154" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C174" t="s">
+    <row r="175" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C175" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C195" t="s">
+    <row r="196" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C196" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="196" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D196" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="197" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D197" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="198" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D198" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="216" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C216" t="s">
+    <row r="217" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C217" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C237" t="s">
+    <row r="238" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C238" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C256" t="s">
+    <row r="257" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C257" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="279" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C279" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="280" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C280" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="281" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C281" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="303" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C303" t="s">
+    <row r="304" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C304" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="304" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D304" t="s">
+    <row r="305" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D305" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="306" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C306" t="s">
+    <row r="307" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C307" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="307" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D307" t="s">
+    <row r="308" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D308" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3860,9 +3869,9 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="4" manualBreakCount="4">
     <brk id="39" max="11" man="1"/>
-    <brk id="79" max="11" man="1"/>
-    <brk id="117" max="11" man="1"/>
-    <brk id="152" max="11" man="1"/>
+    <brk id="80" max="11" man="1"/>
+    <brk id="118" max="11" man="1"/>
+    <brk id="153" max="11" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -3939,7 +3948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U80" sqref="U80"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[DOC] : Version Control Tool_Manual : tortoiseSVN manual 추가
</commit_message>
<xml_diff>
--- a/Version Control Tool_Manual_v1.0.xlsx
+++ b/Version Control Tool_Manual_v1.0.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GitHub 가입" sheetId="13" r:id="rId1"/>
@@ -16,14 +16,14 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Commit Log 확인 방법'!$A$1:$N$147</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'GitHub Local 설정'!$A$1:$L$321</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'GitHub 가입'!$A$1:$P$140</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">TortoiseSVN!$A$1:$P$94</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">TortoiseSVN!$A$1:$P$246</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>5. Repository 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -242,6 +242,62 @@
   </si>
   <si>
     <t>Clone 설정시 Clone folder는 비어 있어야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default 상태로 옵션 선택하여 install 하면 됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. SVN Clone folder를 생성하고, Mouse Popup하여 [SVN Checkout]을 선택한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. Checkout 창에서 [URL of repository]에서 아래와 같이 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[URL of repository]에 SVN repository 경로를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Checkout directory]에 Clone folder의 경로를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Clone folder(1_선도함1_납품서류)에 아래와 같이 .svn folder가 생성되고, Checkout finished 창이 실행된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. Clone folder(1_선도함1_납품서류)에 관리하고자 하는 file들을 Copy 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVN server에만 변경사항들에 대한 모든 history가 저장됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버전 관리할 대상 파일들이 위치하는 folder이다. 변경 사항은 Clone에 저장되지 않는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9. 관리 folder의 변경사항을 SVN repository에 Update하기 위해 Mouse Popup에서 [SVN Commit]을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10. Commit 창에서 commit할 file를 선택하고, 변경사항에 대한 message를 작성 후 OK를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. 아래와 같이 SVN repository로 commit이 진행된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12. commit이 정상적으로 처리된 후 아래와 같은 창이 실행되며, OK를 선택하여 commit을 완료한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVN은 Local SVN server에만 변경사항 hitory 정보가 저장되므로 commmit 후 별도의 Push 단계가 없다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2928,13 +2984,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>596828</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2944,8 +3000,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1123950" y="704850"/>
-          <a:ext cx="7426253" cy="3648075"/>
+          <a:off x="1135132" y="903218"/>
+          <a:ext cx="7454413" cy="3605834"/>
           <a:chOff x="1123950" y="704850"/>
           <a:chExt cx="7426253" cy="3648075"/>
         </a:xfrm>
@@ -3040,75 +3096,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9267825" y="9658349"/>
-          <a:ext cx="1295400" cy="390525"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -3118,8 +3114,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1200150" y="4943475"/>
-          <a:ext cx="4791075" cy="3105150"/>
+          <a:off x="1211332" y="5299213"/>
+          <a:ext cx="4814266" cy="3067878"/>
           <a:chOff x="1200150" y="4943475"/>
           <a:chExt cx="4791075" cy="3105150"/>
         </a:xfrm>
@@ -3215,69 +3211,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>485776</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>120482</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="그림 16"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1085851" y="8505825"/>
-          <a:ext cx="7353300" cy="4616282"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>63518</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3288,7 +3229,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -3318,6 +3259,1071 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>120482</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="그룹 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1097033" y="9026387"/>
+          <a:ext cx="7381460" cy="4561617"/>
+          <a:chOff x="1097033" y="8819322"/>
+          <a:chExt cx="7381460" cy="4561617"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="17" name="그림 16"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1097033" y="8819322"/>
+            <a:ext cx="7381460" cy="4561617"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5990811" y="12991685"/>
+            <a:ext cx="1538080" cy="194228"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3915189" y="12531172"/>
+            <a:ext cx="1538080" cy="194228"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="모서리가 둥근 직사각형 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3313872" y="9039224"/>
+            <a:ext cx="1538080" cy="194228"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>74543</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>115956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>251645</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="그룹 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1143000" y="18760108"/>
+          <a:ext cx="2976623" cy="4364936"/>
+          <a:chOff x="1143000" y="18345978"/>
+          <a:chExt cx="2976623" cy="4364935"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="18" name="그림 17"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1143000" y="18345978"/>
+            <a:ext cx="2976623" cy="4364935"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="모서리가 둥근 직사각형 18"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2114550" y="22375881"/>
+            <a:ext cx="1935646" cy="185945"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>132523</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>406948</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>91063</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="그룹 9"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1192696" y="24160371"/>
+          <a:ext cx="4457143" cy="3685714"/>
+          <a:chOff x="1192696" y="23746240"/>
+          <a:chExt cx="4457143" cy="3685714"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="7" name="그림 6"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1192696" y="23746240"/>
+            <a:ext cx="4457143" cy="3685714"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="모서리가 둥근 직사각형 19"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1410528" y="24289164"/>
+            <a:ext cx="4006298" cy="388040"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="모서리가 둥근 직사각형 21"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1405559" y="24706608"/>
+            <a:ext cx="4006298" cy="388040"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>49697</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>82825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>447261</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>81504</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="26" name="그룹 25"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1118154" y="28459042"/>
+          <a:ext cx="5946911" cy="3104658"/>
+          <a:chOff x="1118154" y="28044912"/>
+          <a:chExt cx="6885485" cy="3594652"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="24" name="그림 23"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1118154" y="28044912"/>
+            <a:ext cx="6885485" cy="3594652"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="모서리가 둥근 직사각형 24"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2876550" y="28811466"/>
+            <a:ext cx="1298713" cy="260491"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>31619</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>71909</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="31" name="그룹 30"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1100076" y="35052000"/>
+          <a:ext cx="5589637" cy="4282110"/>
+          <a:chOff x="1133206" y="32633478"/>
+          <a:chExt cx="6142652" cy="4705764"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="28" name="그림 27"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1133206" y="32633478"/>
+            <a:ext cx="6142652" cy="4705764"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="모서리가 둥근 직사각형 28"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2053258" y="36966525"/>
+            <a:ext cx="2170872" cy="205824"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="모서리가 둥근 직사각형 29"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1639957" y="32687730"/>
+            <a:ext cx="5014290" cy="205824"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>49694</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>621195</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>161066</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="35" name="그룹 34"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1118151" y="32169652"/>
+          <a:ext cx="5433392" cy="2372523"/>
+          <a:chOff x="1118151" y="32583783"/>
+          <a:chExt cx="5956038" cy="2600739"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="33" name="그림 32"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1118151" y="32583783"/>
+            <a:ext cx="5956038" cy="2600739"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="34" name="모서리가 둥근 직사각형 33"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2989193" y="33537524"/>
+            <a:ext cx="3984764" cy="876715"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91109</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>115957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>16679</xdr:colOff>
+      <xdr:row>212</xdr:row>
+      <xdr:rowOff>18430</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="39" name="그룹 38"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1159566" y="39880761"/>
+          <a:ext cx="4787461" cy="4043778"/>
+          <a:chOff x="1159566" y="39880761"/>
+          <a:chExt cx="4787461" cy="4043778"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="36" name="그림 35"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1159566" y="39880761"/>
+            <a:ext cx="4787461" cy="4043778"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="모서리가 둥근 직사각형 36"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1344268" y="40796402"/>
+            <a:ext cx="3194602" cy="219076"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="38" name="모서리가 둥근 직사각형 37"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1322734" y="41967562"/>
+            <a:ext cx="4450244" cy="1143415"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>99391</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>563217</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>41326</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="그림 39"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1167848" y="44403065"/>
+          <a:ext cx="5325717" cy="2443283"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>82826</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>124239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>604630</xdr:colOff>
+      <xdr:row>242</xdr:row>
+      <xdr:rowOff>109338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="그림 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1151283" y="47550456"/>
+          <a:ext cx="5383695" cy="2469881"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3368,7 +4374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3403,7 +4409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3697,7 +4703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D308"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A133" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A181" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
@@ -3881,7 +4887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C118"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A28" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
@@ -3946,10 +4952,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:X71"/>
+  <dimension ref="B2:X230"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U80" sqref="U80"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A205" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="P229" sqref="P229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3959,42 +4965,117 @@
     <col min="24" max="24" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="3:24" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
+    <row r="68" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="3:24" x14ac:dyDescent="0.3">
-      <c r="T68" s="5"/>
-    </row>
     <row r="71" spans="3:24" x14ac:dyDescent="0.3">
-      <c r="T71" s="6"/>
-      <c r="X71" s="6"/>
+      <c r="T71" s="5"/>
+    </row>
+    <row r="74" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="T74" s="6"/>
+      <c r="X74" s="6"/>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C114" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D115" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D116" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C137" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C169" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C192" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C214" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="229" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C229" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="230" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D230" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="42" max="15" man="1"/>
+    <brk id="88" max="15" man="1"/>
+    <brk id="136" max="15" man="1"/>
+  </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="16" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>

<commit_message>
[DOC] : Version Control Tool_Manual : tortoiseSVN manual 수정
</commit_message>
<xml_diff>
--- a/Version Control Tool_Manual_v1.0.xlsx
+++ b/Version Control Tool_Manual_v1.0.xlsx
@@ -18,12 +18,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'GitHub 가입'!$A$1:$P$140</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">TortoiseSVN!$A$1:$P$246</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>5. Repository 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -298,6 +298,10 @@
   </si>
   <si>
     <t>SVN은 Local SVN server에만 변경사항 hitory 정보가 저장되므로 commmit 후 별도의 Push 단계가 없다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clone folder에 파일이 있는 경우, 경고 메시지가 뜬다 - 폴더를 비운 상태에서 진행</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3584,15 +3588,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124239</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>132523</xdr:rowOff>
+      <xdr:colOff>165652</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>149088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>406948</xdr:colOff>
-      <xdr:row>134</xdr:row>
-      <xdr:rowOff>91063</xdr:rowOff>
+      <xdr:colOff>448361</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>107628</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3601,7 +3605,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1192696" y="24160371"/>
+          <a:off x="1234109" y="24384001"/>
           <a:ext cx="4457143" cy="3685714"/>
           <a:chOff x="1192696" y="23746240"/>
           <a:chExt cx="4457143" cy="3685714"/>
@@ -4954,8 +4958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X230"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A205" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="P229" sqref="P229"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A106" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5017,19 +5021,24 @@
         <v>63</v>
       </c>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C114" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D115" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D116" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E117" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[DOC] : Version Control Tool_Manual : manual 수정
</commit_message>
<xml_diff>
--- a/Version Control Tool_Manual_v1.0.xlsx
+++ b/Version Control Tool_Manual_v1.0.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GitHub 가입" sheetId="13" r:id="rId1"/>
     <sheet name="GitHub Local 설정" sheetId="14" r:id="rId2"/>
     <sheet name="Commit Log 확인 방법" sheetId="15" r:id="rId3"/>
     <sheet name="TortoiseSVN" sheetId="16" r:id="rId4"/>
+    <sheet name="TortoiseSVN_사용법" sheetId="17" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Commit Log 확인 방법'!$A$1:$N$147</definedName>
@@ -18,12 +19,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'GitHub 가입'!$A$1:$P$140</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">TortoiseSVN!$A$1:$P$246</definedName>
   </definedNames>
-  <calcPr calcId="144525" calcMode="manual"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>5. Repository 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -302,6 +303,26 @@
   </si>
   <si>
     <t>Clone folder에 파일이 있는 경우, 경고 메시지가 뜬다 - 폴더를 비운 상태에서 진행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 수정 사항 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) TortoiseGit &gt; show log 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) 삭제하고자하는 위치 아래에서 마우스 pop-up후 Reset "master" to this… 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3) Hard를 선택 후 OK 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4) 수정되었던 사항은 모두 삭제되고 Not Versioned Files( xxx debug.cfg)만 남는다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4335,6 +4356,231 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1181100" y="685800"/>
+          <a:ext cx="10344150" cy="4905375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1152525" y="5895975"/>
+          <a:ext cx="10334625" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1171575" y="10315575"/>
+          <a:ext cx="4438650" cy="3143250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1133475" y="13906500"/>
+          <a:ext cx="10353675" cy="4638675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -4624,8 +4870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M121"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R72" sqref="R72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4958,8 +5204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X230"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A106" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A217" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5090,4 +5336,51 @@
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+    <col min="2" max="3" width="4.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Git Credential 설정 추가
</commit_message>
<xml_diff>
--- a/Version Control Tool_Manual_v1.0.xlsx
+++ b/Version Control Tool_Manual_v1.0.xlsx
@@ -4,27 +4,27 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GitHub 가입" sheetId="13" r:id="rId1"/>
     <sheet name="GitHub Local 설정" sheetId="14" r:id="rId2"/>
     <sheet name="Commit Log 확인 방법" sheetId="15" r:id="rId3"/>
-    <sheet name="TortoiseSVN" sheetId="16" r:id="rId4"/>
-    <sheet name="TortoiseSVN_사용법" sheetId="17" r:id="rId5"/>
+    <sheet name="TortoiseGit_사용법" sheetId="17" r:id="rId4"/>
+    <sheet name="TortoiseSVN_설치 및 설정" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Commit Log 확인 방법'!$A$1:$N$147</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'GitHub Local 설정'!$A$1:$L$321</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'GitHub 가입'!$A$1:$P$140</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">TortoiseSVN!$A$1:$P$246</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'TortoiseSVN_설치 및 설정'!$A$1:$P$246</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>5. Repository 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -323,6 +323,30 @@
   </si>
   <si>
     <t>4) 수정되었던 사항은 모두 삭제되고 Not Versioned Files( xxx debug.cfg)만 남는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Git Credential 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push시 마다 뜨는 ID/PW 입력을 한번만 하면 되도록 설정하는 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Repository folder에서 마우스 오른쪽 Pop-up 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TortoiseGit &gt; Settings 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) Git &gt; Credential 선택 후 아래와 같이 Credential helper를 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Window Log-in 정보와 같으면, None으로 선택해도 됨</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3005,1359 +3029,6 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>596828</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="6" name="그룹 5"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1135132" y="903218"/>
-          <a:ext cx="7454413" cy="3605834"/>
-          <a:chOff x="1123950" y="704850"/>
-          <a:chExt cx="7426253" cy="3648075"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="3" name="그림 2"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1123950" y="704850"/>
-            <a:ext cx="7426253" cy="3648075"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6629400" y="3790949"/>
-            <a:ext cx="1295400" cy="390525"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="15" name="그룹 14"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1211332" y="5299213"/>
-          <a:ext cx="4814266" cy="3067878"/>
-          <a:chOff x="1200150" y="4943475"/>
-          <a:chExt cx="4791075" cy="3105150"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="14" name="그림 13"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1200150" y="4943475"/>
-            <a:ext cx="4791075" cy="3105150"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1476375" y="6943724"/>
-            <a:ext cx="2971800" cy="600076"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>63518</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="그림 20"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1123950" y="13716000"/>
-          <a:ext cx="7400925" cy="3749693"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>485776</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>120482</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="그룹 1"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1097033" y="9026387"/>
-          <a:ext cx="7381460" cy="4561617"/>
-          <a:chOff x="1097033" y="8819322"/>
-          <a:chExt cx="7381460" cy="4561617"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="17" name="그림 16"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1097033" y="8819322"/>
-            <a:ext cx="7381460" cy="4561617"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5990811" y="12991685"/>
-            <a:ext cx="1538080" cy="194228"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3915189" y="12531172"/>
-            <a:ext cx="1538080" cy="194228"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="모서리가 둥근 직사각형 12"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3313872" y="9039224"/>
-            <a:ext cx="1538080" cy="194228"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>74543</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>115956</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>251645</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="8" name="그룹 7"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1143000" y="18760108"/>
-          <a:ext cx="2976623" cy="4364936"/>
-          <a:chOff x="1143000" y="18345978"/>
-          <a:chExt cx="2976623" cy="4364935"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="18" name="그림 17"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1143000" y="18345978"/>
-            <a:ext cx="2976623" cy="4364935"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="19" name="모서리가 둥근 직사각형 18"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2114550" y="22375881"/>
-            <a:ext cx="1935646" cy="185945"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>165652</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>149088</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>448361</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>107628</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="10" name="그룹 9"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1234109" y="24384001"/>
-          <a:ext cx="4457143" cy="3685714"/>
-          <a:chOff x="1192696" y="23746240"/>
-          <a:chExt cx="4457143" cy="3685714"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="7" name="그림 6"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1192696" y="23746240"/>
-            <a:ext cx="4457143" cy="3685714"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="20" name="모서리가 둥근 직사각형 19"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1410528" y="24289164"/>
-            <a:ext cx="4006298" cy="388040"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="22" name="모서리가 둥근 직사각형 21"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1405559" y="24706608"/>
-            <a:ext cx="4006298" cy="388040"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>49697</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>82825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>447261</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>81504</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="26" name="그룹 25"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1118154" y="28459042"/>
-          <a:ext cx="5946911" cy="3104658"/>
-          <a:chOff x="1118154" y="28044912"/>
-          <a:chExt cx="6885485" cy="3594652"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="24" name="그림 23"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1118154" y="28044912"/>
-            <a:ext cx="6885485" cy="3594652"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="25" name="모서리가 둥근 직사각형 24"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2876550" y="28811466"/>
-            <a:ext cx="1298713" cy="260491"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>31619</xdr:colOff>
-      <xdr:row>169</xdr:row>
-      <xdr:rowOff>49696</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>71909</xdr:colOff>
-      <xdr:row>189</xdr:row>
-      <xdr:rowOff>190501</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="31" name="그룹 30"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1100076" y="35052000"/>
-          <a:ext cx="5589637" cy="4282110"/>
-          <a:chOff x="1133206" y="32633478"/>
-          <a:chExt cx="6142652" cy="4705764"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="28" name="그림 27"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1133206" y="32633478"/>
-            <a:ext cx="6142652" cy="4705764"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="모서리가 둥근 직사각형 28"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2053258" y="36966525"/>
-            <a:ext cx="2170872" cy="205824"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="30" name="모서리가 둥근 직사각형 29"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1639957" y="32687730"/>
-            <a:ext cx="5014290" cy="205824"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>49694</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>66261</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>621195</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>161066</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="35" name="그룹 34"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1118151" y="32169652"/>
-          <a:ext cx="5433392" cy="2372523"/>
-          <a:chOff x="1118151" y="32583783"/>
-          <a:chExt cx="5956038" cy="2600739"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="33" name="그림 32"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="1118151" y="32583783"/>
-            <a:ext cx="5956038" cy="2600739"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="34" name="모서리가 둥근 직사각형 33"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2989193" y="33537524"/>
-            <a:ext cx="3984764" cy="876715"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>91109</xdr:colOff>
-      <xdr:row>192</xdr:row>
-      <xdr:rowOff>115957</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>16679</xdr:colOff>
-      <xdr:row>212</xdr:row>
-      <xdr:rowOff>18430</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="39" name="그룹 38"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1159566" y="39880761"/>
-          <a:ext cx="4787461" cy="4043778"/>
-          <a:chOff x="1159566" y="39880761"/>
-          <a:chExt cx="4787461" cy="4043778"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="36" name="그림 35"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1159566" y="39880761"/>
-            <a:ext cx="4787461" cy="4043778"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="37" name="모서리가 둥근 직사각형 36"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1344268" y="40796402"/>
-            <a:ext cx="3194602" cy="219076"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="38" name="모서리가 둥근 직사각형 37"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1322734" y="41967562"/>
-            <a:ext cx="4450244" cy="1143415"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>99391</xdr:colOff>
-      <xdr:row>214</xdr:row>
-      <xdr:rowOff>82826</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>563217</xdr:colOff>
-      <xdr:row>226</xdr:row>
-      <xdr:rowOff>41326</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="그림 39"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1167848" y="44403065"/>
-          <a:ext cx="5325717" cy="2443283"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>82826</xdr:colOff>
-      <xdr:row>230</xdr:row>
-      <xdr:rowOff>124239</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>604630</xdr:colOff>
-      <xdr:row>242</xdr:row>
-      <xdr:rowOff>109338</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="그림 41"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1151283" y="47550456"/>
-          <a:ext cx="5383695" cy="2469881"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -4574,6 +3245,1512 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>351488</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>18433</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="그룹 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1162050" y="26098500"/>
+          <a:ext cx="7495238" cy="4933333"/>
+          <a:chOff x="1085850" y="19278600"/>
+          <a:chExt cx="7495238" cy="4933333"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="2" name="그림 1"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1085850" y="19278600"/>
+            <a:ext cx="7495238" cy="4933333"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4695825" y="19840575"/>
+            <a:ext cx="2981325" cy="381000"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="그림 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1181100" y="19954875"/>
+          <a:ext cx="5934075" cy="5419725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>596828</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="그룹 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1135132" y="903218"/>
+          <a:ext cx="7454413" cy="3605834"/>
+          <a:chOff x="1123950" y="704850"/>
+          <a:chExt cx="7426253" cy="3648075"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="그림 2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1123950" y="704850"/>
+            <a:ext cx="7426253" cy="3648075"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6629400" y="3790949"/>
+            <a:ext cx="1295400" cy="390525"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="그룹 14"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1211332" y="5299213"/>
+          <a:ext cx="4814266" cy="3067878"/>
+          <a:chOff x="1200150" y="4943475"/>
+          <a:chExt cx="4791075" cy="3105150"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="14" name="그림 13"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1200150" y="4943475"/>
+            <a:ext cx="4791075" cy="3105150"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1476375" y="6943724"/>
+            <a:ext cx="2971800" cy="600076"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>63518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="그림 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1123950" y="13716000"/>
+          <a:ext cx="7400925" cy="3749693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>120482</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="그룹 1"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1097033" y="9026387"/>
+          <a:ext cx="7381460" cy="4561617"/>
+          <a:chOff x="1097033" y="8819322"/>
+          <a:chExt cx="7381460" cy="4561617"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="17" name="그림 16"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1097033" y="8819322"/>
+            <a:ext cx="7381460" cy="4561617"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5990811" y="12991685"/>
+            <a:ext cx="1538080" cy="194228"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3915189" y="12531172"/>
+            <a:ext cx="1538080" cy="194228"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="모서리가 둥근 직사각형 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3313872" y="9039224"/>
+            <a:ext cx="1538080" cy="194228"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>74543</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>115956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>251645</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="그룹 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1143000" y="18760108"/>
+          <a:ext cx="2976623" cy="4364936"/>
+          <a:chOff x="1143000" y="18345978"/>
+          <a:chExt cx="2976623" cy="4364935"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="18" name="그림 17"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1143000" y="18345978"/>
+            <a:ext cx="2976623" cy="4364935"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="모서리가 둥근 직사각형 18"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2114550" y="22375881"/>
+            <a:ext cx="1935646" cy="185945"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>165652</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>149088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>448361</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>107628</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="그룹 9"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1234109" y="24384001"/>
+          <a:ext cx="4457143" cy="3685714"/>
+          <a:chOff x="1192696" y="23746240"/>
+          <a:chExt cx="4457143" cy="3685714"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="7" name="그림 6"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1192696" y="23746240"/>
+            <a:ext cx="4457143" cy="3685714"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="모서리가 둥근 직사각형 19"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1410528" y="24289164"/>
+            <a:ext cx="4006298" cy="388040"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="모서리가 둥근 직사각형 21"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1405559" y="24706608"/>
+            <a:ext cx="4006298" cy="388040"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>49697</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>82825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>447261</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>81504</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="26" name="그룹 25"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1118154" y="28459042"/>
+          <a:ext cx="5946911" cy="3104658"/>
+          <a:chOff x="1118154" y="28044912"/>
+          <a:chExt cx="6885485" cy="3594652"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="24" name="그림 23"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1118154" y="28044912"/>
+            <a:ext cx="6885485" cy="3594652"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="모서리가 둥근 직사각형 24"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2876550" y="28811466"/>
+            <a:ext cx="1298713" cy="260491"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>31619</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>71909</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="31" name="그룹 30"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1100076" y="35052000"/>
+          <a:ext cx="5589637" cy="4282110"/>
+          <a:chOff x="1133206" y="32633478"/>
+          <a:chExt cx="6142652" cy="4705764"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="28" name="그림 27"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1133206" y="32633478"/>
+            <a:ext cx="6142652" cy="4705764"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="모서리가 둥근 직사각형 28"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2053258" y="36966525"/>
+            <a:ext cx="2170872" cy="205824"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="모서리가 둥근 직사각형 29"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1639957" y="32687730"/>
+            <a:ext cx="5014290" cy="205824"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>49694</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>621195</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>161066</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="35" name="그룹 34"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1118151" y="32169652"/>
+          <a:ext cx="5433392" cy="2372523"/>
+          <a:chOff x="1118151" y="32583783"/>
+          <a:chExt cx="5956038" cy="2600739"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="33" name="그림 32"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="1118151" y="32583783"/>
+            <a:ext cx="5956038" cy="2600739"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="34" name="모서리가 둥근 직사각형 33"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2989193" y="33537524"/>
+            <a:ext cx="3984764" cy="876715"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91109</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>115957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>16679</xdr:colOff>
+      <xdr:row>212</xdr:row>
+      <xdr:rowOff>18430</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="39" name="그룹 38"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1159566" y="39880761"/>
+          <a:ext cx="4787461" cy="4043778"/>
+          <a:chOff x="1159566" y="39880761"/>
+          <a:chExt cx="4787461" cy="4043778"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="36" name="그림 35"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1159566" y="39880761"/>
+            <a:ext cx="4787461" cy="4043778"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="모서리가 둥근 직사각형 36"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1344268" y="40796402"/>
+            <a:ext cx="3194602" cy="219076"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="38" name="모서리가 둥근 직사각형 37"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1322734" y="41967562"/>
+            <a:ext cx="4450244" cy="1143415"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>99391</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>563217</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>41326</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="그림 39"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1167848" y="44403065"/>
+          <a:ext cx="5325717" cy="2443283"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>82826</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>124239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>604630</xdr:colOff>
+      <xdr:row>242</xdr:row>
+      <xdr:rowOff>109338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="그림 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1151283" y="47550456"/>
+          <a:ext cx="5383695" cy="2469881"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -4870,7 +5047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M121"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R72" sqref="R72"/>
     </sheetView>
   </sheetViews>
@@ -4953,7 +5130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D308"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A181" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A70" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
@@ -5137,7 +5314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C118"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A28" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
@@ -5202,10 +5379,87 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D124"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="Q100" sqref="Q100"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+    <col min="2" max="3" width="4.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B91" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C92" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C94" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D95" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C123" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D124" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X230"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A217" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5336,51 +5590,4 @@
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C66"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.75" customWidth="1"/>
-    <col min="2" max="3" width="4.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C28" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C66" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[Manual] Tortoisegit 설치 메뉴얼 추가
</commit_message>
<xml_diff>
--- a/Version Control Tool_Manual_v1.0.xlsx
+++ b/Version Control Tool_Manual_v1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>5. Repository 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -364,6 +364,30 @@
   </si>
   <si>
     <t>2. Windows에 맞는 Program을 download 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Program 실행하면 아래와 같은 화면이 출력되며,  Next를 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 아래와 같이 선택 후 Next를 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 기본 상태에서 Next를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. install  선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Finish 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. first start wizard 설정 - 아래 순서대로 선택한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -881,6 +905,424 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>233030</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1095375" y="10163175"/>
+          <a:ext cx="3862055" cy="3019425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>175880</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5153025" y="10153650"/>
+          <a:ext cx="3862055" cy="3019425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="그림 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1076325" y="13687425"/>
+          <a:ext cx="3876675" cy="3030855"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>72217</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="그림 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5495925" y="13716000"/>
+          <a:ext cx="3990975" cy="3120217"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>66850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1047750" y="17287876"/>
+          <a:ext cx="3971925" cy="3105324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>159502</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="그림 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5591175" y="17268826"/>
+          <a:ext cx="4114800" cy="3217026"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330940</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1057275" y="20840700"/>
+          <a:ext cx="3998065" cy="3571875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>159490</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="그림 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5686425" y="20802600"/>
+          <a:ext cx="3998065" cy="3571875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>359515</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="그림 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1085850" y="24679275"/>
+          <a:ext cx="3998065" cy="3571875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>130915</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="그림 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5657850" y="24641175"/>
+          <a:ext cx="3998065" cy="3571875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>118507</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="그림 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1085850" y="28413075"/>
+          <a:ext cx="3981450" cy="3557032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5260,24 +5702,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="N148" sqref="N148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="4.25" customWidth="1"/>
+    <col min="1" max="1" width="4.25" customWidth="1"/>
+    <col min="2" max="3" width="4.25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -5287,8 +5731,34 @@
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C65" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C82" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C99" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>